<commit_message>
Hoàn thiện tính năng lọc sản phẩm và file automation test của lọc, có sự điều chỉnh ở Homecontroller, ProductDao, ProductService, ProductServeceImpl, có điều chỉnh applicatone để kết nối dtb
</commit_message>
<xml_diff>
--- a/src/test/resources/TestSearchFilterData.xlsx
+++ b/src/test/resources/TestSearchFilterData.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\asm-ktnc\asmkiemthu\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPOLY\2025\FALL\JAVA3\eclipse-workspace\asmkiemthu\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F87BF13-9157-4D39-93D1-1C8B0EA0A14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21249338-7B4E-4A1F-BB4D-94E071D1E797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="1500" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_case" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -96,74 +91,35 @@
     <t>Test Dropdown sắp xếp</t>
   </si>
   <si>
+    <t>Giày NBAL Special Edition</t>
+  </si>
+  <si>
+    <t>Thành công: 8 SP</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
+    <t>Lỗi: Không tìm thấy sản phẩm</t>
+  </si>
+  <si>
     <t>FAIL</t>
   </si>
   <si>
-    <t>Thành công: 31 SP</t>
-  </si>
-  <si>
-    <t>Lỗi: Vẫn hiển thị 7 SP</t>
-  </si>
-  <si>
-    <t>Lỗi hệ thống: Expected condition failed: waiting for presence of element located by: By.xpath: //a[contains(text(),'Adidas')] | //span[contains(text(),'Adidas')] (tried for 10 second(s) with 500 milliseconds interval)</t>
-  </si>
-  <si>
-    <t>Lỗi hệ thống: Expected condition failed: waiting for presence of element located by: By.xpath: //a[contains(text(),'Nike')] | //span[contains(text(),'Nike')] (tried for 10 second(s) with 500 milliseconds interval)</t>
-  </si>
-  <si>
-    <t>Giày NBAL Special Edition</t>
-  </si>
-  <si>
-    <t>Lỗi hệ thống: invalid session id: session deleted as the browser has closed the connection
-from disconnected: not connected to DevTools
-  (Session info: chrome=145.0.7632.76)
+    <t>Đúng: 0 kết quả</t>
+  </si>
+  <si>
+    <t>Lỗi hệ thống: Cannot locate option with text: Tất cả hãng
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
 Build info: version: '4.14.1', revision: '03f8ede370'
-System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [fead67d04691a919fe6942091e31c779, findElements {using=xpath, value=//div[contains(@class, 'card')] | //div[@class='product-item']}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.76, chrome: {chromedriverVersion: 145.0.7632.77 (da516187054a..., userDataDir: C:\Users\DELL\AppData\Local...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50460}, goog:processID: 20504, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50460/devtoo..., se:cdpVersion: 145.0.7632.76, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: fead67d04691a919fe6942091e31c779</t>
-  </si>
-  <si>
-    <t>Lỗi hệ thống: invalid session id: session deleted as the browser has closed the connection
-from disconnected: not connected to DevTools
-  (Session info: chrome=145.0.7632.76)
-Build info: version: '4.14.1', revision: '03f8ede370'
-System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [1eb7cbb64515be24d27e218189623961, findElements {using=xpath, value=//div[contains(@class, 'card')] | //div[@class='product-item']}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.76, chrome: {chromedriverVersion: 145.0.7632.77 (da516187054a..., userDataDir: C:\Users\DELL\AppData\Local...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50499}, goog:processID: 21492, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50499/devtoo..., se:cdpVersion: 145.0.7632.76, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 1eb7cbb64515be24d27e218189623961</t>
-  </si>
-  <si>
-    <t>Lỗi hệ thống: invalid session id: session deleted as the browser has closed the connection
-from disconnected: not connected to DevTools
-  (Session info: chrome=145.0.7632.76)
-Build info: version: '4.14.1', revision: '03f8ede370'
-System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [eff75482d3215d0f49e7dcc4b42469e6, findElement {using=xpath, value=//a[contains(text(),'Nike')] | //span[contains(text(),'Nike')]}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 145.0.7632.76, chrome: {chromedriverVersion: 145.0.7632.77 (da516187054a..., userDataDir: C:\Users\DELL\AppData\Local...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50647}, goog:processID: 20164, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50647/devtoo..., se:cdpVersion: 145.0.7632.76, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: eff75482d3215d0f49e7dcc4b42469e6</t>
-  </si>
-  <si>
-    <t>Thành công: 13 SP</t>
-  </si>
-  <si>
-    <t>Thành công: 7 SP</t>
-  </si>
-  <si>
-    <t>Thành công: 5 SP</t>
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: driver.version: unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -221,8 +177,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -453,14 +409,14 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="20.0"/>
-    <col min="6" max="6" customWidth="true" width="31.36328125"/>
-    <col min="7" max="7" customWidth="true" width="41.36328125"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="6" max="6" width="31.36328125" customWidth="1"/>
+    <col min="7" max="7" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -498,11 +454,11 @@
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>23</v>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -510,7 +466,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -520,11 +476,11 @@
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>23</v>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -542,11 +498,11 @@
       <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>24</v>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -564,11 +520,11 @@
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>23</v>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -586,11 +542,11 @@
       <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>23</v>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -598,8 +554,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -608,11 +563,11 @@
       <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>23</v>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -630,11 +585,11 @@
       <c r="F8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>24</v>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -652,11 +607,11 @@
       <c r="F9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G9" t="s" s="0">
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
         <v>25</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>